<commit_message>
add custom hook to fetch data from server
</commit_message>
<xml_diff>
--- a/backend/design.xlsx
+++ b/backend/design.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\programming\learning\coursera_back_end_developer_course_by_meta\course_6_APIs\_Exercises\week3\LittleLemonAPI_Final_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\programming\learning\react\other_projects_and_resources\projects\little_lemon_restaurant\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -261,12 +261,6 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -290,6 +284,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,29 +578,29 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A3:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScale="60" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" customWidth="1"/>
-    <col min="8" max="8" width="6.109375" style="10" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" style="10" customWidth="1"/>
+    <col min="8" max="8" width="8" style="8" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -608,11 +608,11 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
@@ -630,7 +630,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="9" t="s">
         <v>34</v>
       </c>
       <c r="B11" t="s">
@@ -638,31 +638,31 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="1" t="s">
         <v>31</v>
       </c>
     </row>
@@ -676,44 +676,46 @@
       <c r="D13" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="8">
         <v>201</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="13" t="s">
         <v>32</v>
       </c>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G14" s="2"/>
-      <c r="H14" s="10">
+      <c r="G14" s="12"/>
+      <c r="H14" s="8">
         <v>404</v>
       </c>
-      <c r="I14" s="10" t="s">
+      <c r="I14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G15" s="2"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+      <c r="G15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
     </row>
     <row r="16" spans="1:12" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -722,24 +724,24 @@
       <c r="C16" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="8">
         <v>200</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="I16" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F17" s="7"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
@@ -748,24 +750,24 @@
       <c r="C18" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H18" s="8">
         <v>200</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I18" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B21" t="s">
@@ -777,19 +779,19 @@
       <c r="D21" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="10">
+      <c r="H21" s="8">
         <v>200</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J21" t="s">
@@ -800,19 +802,19 @@
       <c r="D22" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H22" s="10">
+      <c r="H22" s="8">
         <v>200</v>
       </c>
-      <c r="I22" s="10" t="s">
+      <c r="I22" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J22" t="s">
@@ -823,19 +825,19 @@
       <c r="D23" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G23" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H23" s="10">
+      <c r="H23" s="8">
         <v>200</v>
       </c>
-      <c r="I23" s="10" t="s">
+      <c r="I23" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J23" t="s">
@@ -846,19 +848,19 @@
       <c r="D24" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H24" s="8">
         <v>201</v>
       </c>
-      <c r="I24" s="10" t="s">
+      <c r="I24" s="8" t="s">
         <v>17</v>
       </c>
       <c r="J24" t="s">
@@ -866,7 +868,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B26" t="s">
@@ -878,13 +880,13 @@
       <c r="D26" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="G26" s="11" t="s">
         <v>47</v>
       </c>
     </row>
@@ -892,13 +894,13 @@
       <c r="D27" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="11" t="s">
         <v>47</v>
       </c>
     </row>
@@ -906,13 +908,13 @@
       <c r="D28" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="11" t="s">
         <v>47</v>
       </c>
     </row>
@@ -920,13 +922,13 @@
       <c r="D29" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G29" s="13" t="s">
+      <c r="G29" s="11" t="s">
         <v>52</v>
       </c>
     </row>
@@ -934,13 +936,13 @@
       <c r="D30" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="G30" s="11" t="s">
         <v>51</v>
       </c>
     </row>
@@ -948,13 +950,13 @@
       <c r="D31" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="G31" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -964,7 +966,7 @@
     <mergeCell ref="J14:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="93" orientation="landscape" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="A11 A21 A26" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>